<commit_message>
version completa web febrero 2021
</commit_message>
<xml_diff>
--- a/Files/Reporte_Kardex/1/Kardex_suc_1.xlsx
+++ b/Files/Reporte_Kardex/1/Kardex_suc_1.xlsx
@@ -15,9 +15,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
-  <si>
-    <t>Estuche Ringke Fusion X Apple Iphone 7/8 - Negro</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+  <si>
+    <t>Estuche Spigen Liquid Air Apple iPhone XR - Negro</t>
   </si>
   <si>
     <t>CODIGO</t>
@@ -26,13 +26,13 @@
     <t>UBICACIÓN</t>
   </si>
   <si>
-    <t>7B</t>
+    <t>3C</t>
   </si>
   <si>
     <t>SKU</t>
   </si>
   <si>
-    <t>IGSG0011</t>
+    <t>064CS24872</t>
   </si>
   <si>
     <t>EXISTENCIA</t>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>SALIDAS</t>
+  </si>
+  <si>
+    <t>Cargue Inicial</t>
   </si>
 </sst>
 </file>
@@ -484,10 +487,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -510,7 +513,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4">
-        <v>8809628565333</v>
+        <v>8809613763935</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
@@ -532,7 +535,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="1">
-        <v>37</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" customHeight="1" ht="25">
@@ -554,13 +557,13 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="8">
-        <v>44139</v>
+        <v>44221</v>
       </c>
       <c r="B5" s="7">
-        <v>0.82565972222222</v>
+        <v>0.44732638888889</v>
       </c>
       <c r="C5">
-        <v>300098762</v>
+        <v>4173011669</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="6">
@@ -569,46 +572,18 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="8">
-        <v>44139</v>
+        <v>44221</v>
       </c>
       <c r="B6" s="7">
-        <v>0.77010416666667</v>
-      </c>
-      <c r="C6">
-        <v>302159019</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="8">
-        <v>44139</v>
-      </c>
-      <c r="B7" s="7">
-        <v>0.77008101851852</v>
-      </c>
-      <c r="C7">
-        <v>302158968</v>
-      </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="8">
-        <v>44139</v>
-      </c>
-      <c r="B8" s="7">
-        <v>0.60262731481481</v>
-      </c>
-      <c r="C8"/>
-      <c r="D8" s="5">
-        <v>40</v>
-      </c>
-      <c r="E8" s="6"/>
+        <v>0.44269675925926</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="5">
+        <v>6</v>
+      </c>
+      <c r="E6" s="6"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>